<commit_message>
2.0 begin （A1 ing）
</commit_message>
<xml_diff>
--- a/PatternNumber.xlsx
+++ b/PatternNumber.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="0" windowWidth="19320" windowHeight="9465" activeTab="1"/>
+    <workbookView xWindow="3360" yWindow="0" windowWidth="19320" windowHeight="9465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2915,10 +2915,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM41"/>
+  <dimension ref="A1:AN57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AJ12" sqref="AJ12"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="AU11" sqref="AU11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2926,7 +2926,7 @@
     <col min="1" max="56" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3">
         <v>1</v>
       </c>
@@ -3010,8 +3010,35 @@
       <c r="AC1" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE1" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF1" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG1" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH1" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI1" s="3">
+        <v>5</v>
+      </c>
+      <c r="AJ1" s="3">
+        <v>6</v>
+      </c>
+      <c r="AK1" s="3">
+        <v>7</v>
+      </c>
+      <c r="AL1" s="3">
+        <v>8</v>
+      </c>
+      <c r="AM1" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>10</v>
       </c>
@@ -3052,7 +3079,7 @@
       <c r="N2" s="3">
         <v>13</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="3">
         <v>14</v>
       </c>
       <c r="P2" s="3">
@@ -3080,7 +3107,7 @@
       <c r="X2" s="3">
         <v>13</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2" s="3">
         <v>14</v>
       </c>
       <c r="Z2" s="3">
@@ -3095,8 +3122,35 @@
       <c r="AC2" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE2" s="3">
+        <v>10</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>11</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>12</v>
+      </c>
+      <c r="AH2" s="3">
+        <v>13</v>
+      </c>
+      <c r="AI2" s="3">
+        <v>14</v>
+      </c>
+      <c r="AJ2" s="3">
+        <v>15</v>
+      </c>
+      <c r="AK2" s="3">
+        <v>16</v>
+      </c>
+      <c r="AL2" s="3">
+        <v>17</v>
+      </c>
+      <c r="AM2" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>19</v>
       </c>
@@ -3159,19 +3213,19 @@
       <c r="V3" s="3">
         <v>20</v>
       </c>
-      <c r="W3" s="3">
+      <c r="W3" s="2">
         <v>21</v>
       </c>
-      <c r="X3" s="3">
+      <c r="X3" s="2">
         <v>22</v>
       </c>
       <c r="Y3" s="2">
         <v>23</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="Z3" s="2">
         <v>24</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AA3" s="2">
         <v>25</v>
       </c>
       <c r="AB3" s="3">
@@ -3180,8 +3234,35 @@
       <c r="AC3" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE3" s="3">
+        <v>19</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>20</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>21</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>22</v>
+      </c>
+      <c r="AI3" s="3">
+        <v>23</v>
+      </c>
+      <c r="AJ3" s="3">
+        <v>24</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>25</v>
+      </c>
+      <c r="AL3" s="3">
+        <v>26</v>
+      </c>
+      <c r="AM3" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>28</v>
       </c>
@@ -3250,7 +3331,7 @@
       <c r="X4" s="3">
         <v>31</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Y4" s="3">
         <v>32</v>
       </c>
       <c r="Z4" s="3">
@@ -3265,12 +3346,39 @@
       <c r="AC4" s="3">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE4" s="3">
+        <v>28</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>29</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>30</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>31</v>
+      </c>
+      <c r="AI4" s="3">
+        <v>32</v>
+      </c>
+      <c r="AJ4" s="3">
+        <v>33</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>34</v>
+      </c>
+      <c r="AL4" s="3">
+        <v>35</v>
+      </c>
+      <c r="AM4" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>37</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>38</v>
       </c>
       <c r="C5" s="2">
@@ -3288,7 +3396,7 @@
       <c r="G5" s="2">
         <v>43</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>44</v>
       </c>
       <c r="I5" s="3">
@@ -3326,32 +3434,59 @@
       <c r="U5" s="3">
         <v>37</v>
       </c>
-      <c r="V5" s="2">
+      <c r="V5" s="3">
         <v>38</v>
       </c>
-      <c r="W5" s="2">
+      <c r="W5" s="3">
         <v>39</v>
       </c>
-      <c r="X5" s="2">
+      <c r="X5" s="3">
         <v>40</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Y5" s="3">
         <v>41</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="Z5" s="3">
         <v>42</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AA5" s="3">
         <v>43</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AB5" s="3">
         <v>44</v>
       </c>
       <c r="AC5" s="3">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE5" s="3">
+        <v>37</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>38</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>39</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>40</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>41</v>
+      </c>
+      <c r="AJ5" s="3">
+        <v>42</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL5" s="3">
+        <v>44</v>
+      </c>
+      <c r="AM5" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>46</v>
       </c>
@@ -3420,7 +3555,7 @@
       <c r="X6" s="3">
         <v>49</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Y6" s="3">
         <v>50</v>
       </c>
       <c r="Z6" s="3">
@@ -3435,8 +3570,35 @@
       <c r="AC6" s="3">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE6" s="3">
+        <v>46</v>
+      </c>
+      <c r="AF6" s="3">
+        <v>47</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH6" s="3">
+        <v>49</v>
+      </c>
+      <c r="AI6" s="3">
+        <v>50</v>
+      </c>
+      <c r="AJ6" s="3">
+        <v>51</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>52</v>
+      </c>
+      <c r="AL6" s="3">
+        <v>53</v>
+      </c>
+      <c r="AM6" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>55</v>
       </c>
@@ -3499,19 +3661,19 @@
       <c r="V7" s="3">
         <v>56</v>
       </c>
-      <c r="W7" s="3">
+      <c r="W7" s="2">
         <v>57</v>
       </c>
-      <c r="X7" s="3">
+      <c r="X7" s="2">
         <v>58</v>
       </c>
       <c r="Y7" s="2">
         <v>59</v>
       </c>
-      <c r="Z7" s="3">
+      <c r="Z7" s="2">
         <v>60</v>
       </c>
-      <c r="AA7" s="3">
+      <c r="AA7" s="2">
         <v>61</v>
       </c>
       <c r="AB7" s="3">
@@ -3520,8 +3682,35 @@
       <c r="AC7" s="3">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE7" s="3">
+        <v>55</v>
+      </c>
+      <c r="AF7" s="3">
+        <v>56</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>57</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>58</v>
+      </c>
+      <c r="AI7" s="3">
+        <v>59</v>
+      </c>
+      <c r="AJ7" s="3">
+        <v>60</v>
+      </c>
+      <c r="AK7" s="2">
+        <v>61</v>
+      </c>
+      <c r="AL7" s="3">
+        <v>62</v>
+      </c>
+      <c r="AM7" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>64</v>
       </c>
@@ -3562,7 +3751,7 @@
       <c r="N8" s="3">
         <v>67</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="3">
         <v>68</v>
       </c>
       <c r="P8" s="3">
@@ -3590,7 +3779,7 @@
       <c r="X8" s="3">
         <v>67</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="Y8" s="3">
         <v>68</v>
       </c>
       <c r="Z8" s="3">
@@ -3605,8 +3794,35 @@
       <c r="AC8" s="3">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE8" s="3">
+        <v>64</v>
+      </c>
+      <c r="AF8" s="3">
+        <v>65</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>66</v>
+      </c>
+      <c r="AH8" s="3">
+        <v>67</v>
+      </c>
+      <c r="AI8" s="3">
+        <v>68</v>
+      </c>
+      <c r="AJ8" s="3">
+        <v>69</v>
+      </c>
+      <c r="AK8" s="3">
+        <v>70</v>
+      </c>
+      <c r="AL8" s="3">
+        <v>71</v>
+      </c>
+      <c r="AM8" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>73</v>
       </c>
@@ -3690,8 +3906,35 @@
       <c r="AC9" s="3">
         <v>81</v>
       </c>
-    </row>
-    <row r="10" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE9" s="3">
+        <v>73</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>74</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>75</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>76</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>77</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>78</v>
+      </c>
+      <c r="AK9" s="3">
+        <v>79</v>
+      </c>
+      <c r="AL9" s="3">
+        <v>80</v>
+      </c>
+      <c r="AM9" s="3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -3722,7 +3965,7 @@
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
     </row>
-    <row r="11" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -3806,6 +4049,7 @@
       <c r="AC11" s="3">
         <v>9</v>
       </c>
+      <c r="AD11" s="4"/>
       <c r="AE11" s="3">
         <v>1</v>
       </c>
@@ -3833,8 +4077,9 @@
       <c r="AM11" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN11" s="4"/>
+    </row>
+    <row r="12" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -3847,7 +4092,7 @@
       <c r="D12" s="3">
         <v>13</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>14</v>
       </c>
       <c r="F12" s="3">
@@ -3903,7 +4148,7 @@
       <c r="X12" s="3">
         <v>13</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="Y12" s="3">
         <v>14</v>
       </c>
       <c r="Z12" s="3">
@@ -3918,6 +4163,7 @@
       <c r="AC12" s="3">
         <v>18</v>
       </c>
+      <c r="AD12" s="4"/>
       <c r="AE12" s="3">
         <v>10</v>
       </c>
@@ -3930,7 +4176,7 @@
       <c r="AH12" s="3">
         <v>13</v>
       </c>
-      <c r="AI12" s="2">
+      <c r="AI12" s="3">
         <v>14</v>
       </c>
       <c r="AJ12" s="3">
@@ -3945,21 +4191,22 @@
       <c r="AM12" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN12" s="4"/>
+    </row>
+    <row r="13" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>19</v>
       </c>
       <c r="B13" s="3">
         <v>20</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>21</v>
       </c>
       <c r="D13" s="3">
         <v>22</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>23</v>
       </c>
       <c r="F13" s="3">
@@ -3993,7 +4240,7 @@
       <c r="P13" s="3">
         <v>24</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="Q13" s="2">
         <v>25</v>
       </c>
       <c r="R13" s="3">
@@ -4009,19 +4256,19 @@
       <c r="V13" s="3">
         <v>20</v>
       </c>
-      <c r="W13" s="3">
+      <c r="W13" s="2">
         <v>21</v>
       </c>
-      <c r="X13" s="3">
+      <c r="X13" s="2">
         <v>22</v>
       </c>
       <c r="Y13" s="2">
         <v>23</v>
       </c>
-      <c r="Z13" s="3">
+      <c r="Z13" s="2">
         <v>24</v>
       </c>
-      <c r="AA13" s="3">
+      <c r="AA13" s="2">
         <v>25</v>
       </c>
       <c r="AB13" s="3">
@@ -4030,25 +4277,26 @@
       <c r="AC13" s="3">
         <v>27</v>
       </c>
+      <c r="AD13" s="4"/>
       <c r="AE13" s="3">
         <v>19</v>
       </c>
       <c r="AF13" s="3">
         <v>20</v>
       </c>
-      <c r="AG13" s="3">
+      <c r="AG13" s="2">
         <v>21</v>
       </c>
-      <c r="AH13" s="3">
+      <c r="AH13" s="2">
         <v>22</v>
       </c>
       <c r="AI13" s="2">
         <v>23</v>
       </c>
-      <c r="AJ13" s="3">
+      <c r="AJ13" s="2">
         <v>24</v>
       </c>
-      <c r="AK13" s="3">
+      <c r="AK13" s="2">
         <v>25</v>
       </c>
       <c r="AL13" s="3">
@@ -4057,21 +4305,22 @@
       <c r="AM13" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN13" s="4"/>
+    </row>
+    <row r="14" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>28</v>
       </c>
       <c r="B14" s="3">
         <v>29</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>30</v>
       </c>
       <c r="D14" s="3">
         <v>31</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="3">
         <v>32</v>
       </c>
       <c r="F14" s="3">
@@ -4105,7 +4354,7 @@
       <c r="P14" s="3">
         <v>33</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="Q14" s="2">
         <v>34</v>
       </c>
       <c r="R14" s="3">
@@ -4121,13 +4370,13 @@
       <c r="V14" s="3">
         <v>29</v>
       </c>
-      <c r="W14" s="3">
+      <c r="W14" s="2">
         <v>30</v>
       </c>
       <c r="X14" s="3">
         <v>31</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="Y14" s="3">
         <v>32</v>
       </c>
       <c r="Z14" s="3">
@@ -4142,6 +4391,7 @@
       <c r="AC14" s="3">
         <v>36</v>
       </c>
+      <c r="AD14" s="4"/>
       <c r="AE14" s="3">
         <v>28</v>
       </c>
@@ -4154,13 +4404,13 @@
       <c r="AH14" s="3">
         <v>31</v>
       </c>
-      <c r="AI14" s="2">
+      <c r="AI14" s="3">
         <v>32</v>
       </c>
       <c r="AJ14" s="3">
         <v>33</v>
       </c>
-      <c r="AK14" s="3">
+      <c r="AK14" s="2">
         <v>34</v>
       </c>
       <c r="AL14" s="3">
@@ -4169,30 +4419,31 @@
       <c r="AM14" s="3">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN14" s="4"/>
+    </row>
+    <row r="15" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>37</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>38</v>
       </c>
       <c r="C15" s="2">
         <v>39</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="3">
         <v>40</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <v>41</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="3">
         <v>42</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="3">
         <v>43</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="3">
         <v>44</v>
       </c>
       <c r="I15" s="3">
@@ -4202,25 +4453,25 @@
       <c r="K15" s="3">
         <v>37</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="3">
         <v>38</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="3">
         <v>39</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="3">
         <v>40</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O15" s="3">
         <v>41</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="3">
         <v>42</v>
       </c>
       <c r="Q15" s="2">
         <v>43</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15" s="3">
         <v>44</v>
       </c>
       <c r="S15" s="3">
@@ -4230,16 +4481,16 @@
       <c r="U15" s="3">
         <v>37</v>
       </c>
-      <c r="V15" s="2">
+      <c r="V15" s="3">
         <v>38</v>
       </c>
       <c r="W15" s="2">
         <v>39</v>
       </c>
-      <c r="X15" s="2">
+      <c r="X15" s="3">
         <v>40</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="Y15" s="3">
         <v>41</v>
       </c>
       <c r="Z15" s="3">
@@ -4254,6 +4505,7 @@
       <c r="AC15" s="3">
         <v>45</v>
       </c>
+      <c r="AD15" s="4"/>
       <c r="AE15" s="3">
         <v>37</v>
       </c>
@@ -4266,30 +4518,31 @@
       <c r="AH15" s="3">
         <v>40</v>
       </c>
-      <c r="AI15" s="2">
+      <c r="AI15" s="3">
         <v>41</v>
       </c>
-      <c r="AJ15" s="2">
+      <c r="AJ15" s="3">
         <v>42</v>
       </c>
       <c r="AK15" s="2">
         <v>43</v>
       </c>
-      <c r="AL15" s="2">
+      <c r="AL15" s="3">
         <v>44</v>
       </c>
       <c r="AM15" s="3">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN15" s="4"/>
+    </row>
+    <row r="16" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>46</v>
       </c>
       <c r="B16" s="3">
         <v>47</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>48</v>
       </c>
       <c r="D16" s="3">
@@ -4323,13 +4576,13 @@
       <c r="N16" s="3">
         <v>49</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="3">
         <v>50</v>
       </c>
       <c r="P16" s="3">
         <v>51</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="Q16" s="2">
         <v>52</v>
       </c>
       <c r="R16" s="3">
@@ -4345,13 +4598,13 @@
       <c r="V16" s="3">
         <v>47</v>
       </c>
-      <c r="W16" s="3">
+      <c r="W16" s="2">
         <v>48</v>
       </c>
       <c r="X16" s="3">
         <v>49</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="Y16" s="3">
         <v>50</v>
       </c>
       <c r="Z16" s="3">
@@ -4366,6 +4619,7 @@
       <c r="AC16" s="3">
         <v>54</v>
       </c>
+      <c r="AD16" s="4"/>
       <c r="AE16" s="3">
         <v>46</v>
       </c>
@@ -4378,13 +4632,13 @@
       <c r="AH16" s="3">
         <v>49</v>
       </c>
-      <c r="AI16" s="2">
+      <c r="AI16" s="3">
         <v>50</v>
       </c>
       <c r="AJ16" s="3">
         <v>51</v>
       </c>
-      <c r="AK16" s="3">
+      <c r="AK16" s="2">
         <v>52</v>
       </c>
       <c r="AL16" s="3">
@@ -4393,27 +4647,28 @@
       <c r="AM16" s="3">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN16" s="4"/>
+    </row>
+    <row r="17" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>55</v>
       </c>
       <c r="B17" s="3">
         <v>56</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>57</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>58</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>59</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>60</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
         <v>61</v>
       </c>
       <c r="H17" s="3">
@@ -4429,19 +4684,19 @@
       <c r="L17" s="3">
         <v>56</v>
       </c>
-      <c r="M17" s="3">
+      <c r="M17" s="2">
         <v>57</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17" s="2">
         <v>58</v>
       </c>
       <c r="O17" s="2">
         <v>59</v>
       </c>
-      <c r="P17" s="3">
+      <c r="P17" s="2">
         <v>60</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="Q17" s="2">
         <v>61</v>
       </c>
       <c r="R17" s="3">
@@ -4457,13 +4712,13 @@
       <c r="V17" s="3">
         <v>56</v>
       </c>
-      <c r="W17" s="3">
+      <c r="W17" s="2">
         <v>57</v>
       </c>
       <c r="X17" s="3">
         <v>58</v>
       </c>
-      <c r="Y17" s="2">
+      <c r="Y17" s="3">
         <v>59</v>
       </c>
       <c r="Z17" s="3">
@@ -4478,6 +4733,7 @@
       <c r="AC17" s="3">
         <v>63</v>
       </c>
+      <c r="AD17" s="4"/>
       <c r="AE17" s="3">
         <v>55</v>
       </c>
@@ -4490,13 +4746,13 @@
       <c r="AH17" s="3">
         <v>58</v>
       </c>
-      <c r="AI17" s="2">
+      <c r="AI17" s="3">
         <v>59</v>
       </c>
       <c r="AJ17" s="3">
         <v>60</v>
       </c>
-      <c r="AK17" s="3">
+      <c r="AK17" s="2">
         <v>61</v>
       </c>
       <c r="AL17" s="3">
@@ -4505,8 +4761,9 @@
       <c r="AM17" s="3">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN17" s="4"/>
+    </row>
+    <row r="18" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>64</v>
       </c>
@@ -4547,7 +4804,7 @@
       <c r="N18" s="3">
         <v>67</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O18" s="3">
         <v>68</v>
       </c>
       <c r="P18" s="3">
@@ -4575,7 +4832,7 @@
       <c r="X18" s="3">
         <v>67</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="Y18" s="3">
         <v>68</v>
       </c>
       <c r="Z18" s="3">
@@ -4590,6 +4847,7 @@
       <c r="AC18" s="3">
         <v>72</v>
       </c>
+      <c r="AD18" s="4"/>
       <c r="AE18" s="3">
         <v>64</v>
       </c>
@@ -4602,7 +4860,7 @@
       <c r="AH18" s="3">
         <v>67</v>
       </c>
-      <c r="AI18" s="2">
+      <c r="AI18" s="3">
         <v>68</v>
       </c>
       <c r="AJ18" s="3">
@@ -4617,8 +4875,9 @@
       <c r="AM18" s="3">
         <v>72</v>
       </c>
-    </row>
-    <row r="19" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN18" s="4"/>
+    </row>
+    <row r="19" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>73</v>
       </c>
@@ -4702,6 +4961,7 @@
       <c r="AC19" s="3">
         <v>81</v>
       </c>
+      <c r="AD19" s="4"/>
       <c r="AE19" s="3">
         <v>73</v>
       </c>
@@ -4729,8 +4989,9 @@
       <c r="AM19" s="3">
         <v>81</v>
       </c>
-    </row>
-    <row r="20" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN19" s="4"/>
+    </row>
+    <row r="20" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -4760,8 +5021,19 @@
       <c r="AA20" s="4"/>
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
-    </row>
-    <row r="21" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="4"/>
+      <c r="AG20" s="4"/>
+      <c r="AH20" s="4"/>
+      <c r="AI20" s="4"/>
+      <c r="AJ20" s="4"/>
+      <c r="AK20" s="4"/>
+      <c r="AL20" s="4"/>
+      <c r="AM20" s="4"/>
+      <c r="AN20" s="4"/>
+    </row>
+    <row r="21" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>1</v>
       </c>
@@ -4845,6 +5117,7 @@
       <c r="AC21" s="3">
         <v>9</v>
       </c>
+      <c r="AD21" s="4"/>
       <c r="AE21" s="3">
         <v>1</v>
       </c>
@@ -4872,8 +5145,9 @@
       <c r="AM21" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN21" s="4"/>
+    </row>
+    <row r="22" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>10</v>
       </c>
@@ -4886,7 +5160,7 @@
       <c r="D22" s="3">
         <v>13</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="3">
         <v>14</v>
       </c>
       <c r="F22" s="3">
@@ -4914,7 +5188,7 @@
       <c r="N22" s="3">
         <v>13</v>
       </c>
-      <c r="O22" s="2">
+      <c r="O22" s="3">
         <v>14</v>
       </c>
       <c r="P22" s="3">
@@ -4957,6 +5231,7 @@
       <c r="AC22" s="3">
         <v>18</v>
       </c>
+      <c r="AD22" s="4"/>
       <c r="AE22" s="3">
         <v>10</v>
       </c>
@@ -4984,27 +5259,28 @@
       <c r="AM22" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN22" s="4"/>
+    </row>
+    <row r="23" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>19</v>
       </c>
       <c r="B23" s="3">
         <v>20</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>21</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>22</v>
       </c>
       <c r="E23" s="2">
         <v>23</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>24</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>25</v>
       </c>
       <c r="H23" s="3">
@@ -5048,7 +5324,7 @@
       <c r="V23" s="3">
         <v>20</v>
       </c>
-      <c r="W23" s="3">
+      <c r="W23" s="2">
         <v>21</v>
       </c>
       <c r="X23" s="3">
@@ -5069,6 +5345,7 @@
       <c r="AC23" s="3">
         <v>27</v>
       </c>
+      <c r="AD23" s="4"/>
       <c r="AE23" s="3">
         <v>19</v>
       </c>
@@ -5087,7 +5364,7 @@
       <c r="AJ23" s="3">
         <v>24</v>
       </c>
-      <c r="AK23" s="3">
+      <c r="AK23" s="2">
         <v>25</v>
       </c>
       <c r="AL23" s="3">
@@ -5096,8 +5373,9 @@
       <c r="AM23" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN23" s="4"/>
+    </row>
+    <row r="24" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>28</v>
       </c>
@@ -5160,7 +5438,7 @@
       <c r="V24" s="3">
         <v>29</v>
       </c>
-      <c r="W24" s="3">
+      <c r="W24" s="2">
         <v>30</v>
       </c>
       <c r="X24" s="3">
@@ -5181,6 +5459,7 @@
       <c r="AC24" s="3">
         <v>36</v>
       </c>
+      <c r="AD24" s="4"/>
       <c r="AE24" s="3">
         <v>28</v>
       </c>
@@ -5199,7 +5478,7 @@
       <c r="AJ24" s="3">
         <v>33</v>
       </c>
-      <c r="AK24" s="3">
+      <c r="AK24" s="2">
         <v>34</v>
       </c>
       <c r="AL24" s="3">
@@ -5208,18 +5487,19 @@
       <c r="AM24" s="3">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN24" s="4"/>
+    </row>
+    <row r="25" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>37</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="3">
         <v>38</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="3">
         <v>39</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="3">
         <v>40</v>
       </c>
       <c r="E25" s="2">
@@ -5253,13 +5533,13 @@
       <c r="O25" s="2">
         <v>41</v>
       </c>
-      <c r="P25" s="2">
+      <c r="P25" s="3">
         <v>42</v>
       </c>
-      <c r="Q25" s="2">
+      <c r="Q25" s="3">
         <v>43</v>
       </c>
-      <c r="R25" s="2">
+      <c r="R25" s="3">
         <v>44</v>
       </c>
       <c r="S25" s="3">
@@ -5269,7 +5549,7 @@
       <c r="U25" s="3">
         <v>37</v>
       </c>
-      <c r="V25" s="2">
+      <c r="V25" s="3">
         <v>38</v>
       </c>
       <c r="W25" s="2">
@@ -5281,10 +5561,10 @@
       <c r="Y25" s="2">
         <v>41</v>
       </c>
-      <c r="Z25" s="3">
+      <c r="Z25" s="2">
         <v>42</v>
       </c>
-      <c r="AA25" s="3">
+      <c r="AA25" s="2">
         <v>43</v>
       </c>
       <c r="AB25" s="3">
@@ -5293,16 +5573,17 @@
       <c r="AC25" s="3">
         <v>45</v>
       </c>
+      <c r="AD25" s="4"/>
       <c r="AE25" s="3">
         <v>37</v>
       </c>
       <c r="AF25" s="3">
         <v>38</v>
       </c>
-      <c r="AG25" s="3">
+      <c r="AG25" s="2">
         <v>39</v>
       </c>
-      <c r="AH25" s="3">
+      <c r="AH25" s="2">
         <v>40</v>
       </c>
       <c r="AI25" s="2">
@@ -5314,14 +5595,15 @@
       <c r="AK25" s="2">
         <v>43</v>
       </c>
-      <c r="AL25" s="2">
+      <c r="AL25" s="3">
         <v>44</v>
       </c>
       <c r="AM25" s="3">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN25" s="4"/>
+    </row>
+    <row r="26" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>46</v>
       </c>
@@ -5334,7 +5616,7 @@
       <c r="D26" s="3">
         <v>49</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>50</v>
       </c>
       <c r="F26" s="3">
@@ -5362,7 +5644,7 @@
       <c r="N26" s="3">
         <v>49</v>
       </c>
-      <c r="O26" s="3">
+      <c r="O26" s="2">
         <v>50</v>
       </c>
       <c r="P26" s="3">
@@ -5384,13 +5666,13 @@
       <c r="V26" s="3">
         <v>47</v>
       </c>
-      <c r="W26" s="3">
+      <c r="W26" s="2">
         <v>48</v>
       </c>
       <c r="X26" s="3">
         <v>49</v>
       </c>
-      <c r="Y26" s="2">
+      <c r="Y26" s="3">
         <v>50</v>
       </c>
       <c r="Z26" s="3">
@@ -5405,6 +5687,7 @@
       <c r="AC26" s="3">
         <v>54</v>
       </c>
+      <c r="AD26" s="4"/>
       <c r="AE26" s="3">
         <v>46</v>
       </c>
@@ -5417,13 +5700,13 @@
       <c r="AH26" s="3">
         <v>49</v>
       </c>
-      <c r="AI26" s="2">
+      <c r="AI26" s="3">
         <v>50</v>
       </c>
       <c r="AJ26" s="3">
         <v>51</v>
       </c>
-      <c r="AK26" s="3">
+      <c r="AK26" s="2">
         <v>52</v>
       </c>
       <c r="AL26" s="3">
@@ -5432,8 +5715,9 @@
       <c r="AM26" s="3">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN26" s="4"/>
+    </row>
+    <row r="27" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>55</v>
       </c>
@@ -5446,7 +5730,7 @@
       <c r="D27" s="3">
         <v>58</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>59</v>
       </c>
       <c r="F27" s="3">
@@ -5468,19 +5752,19 @@
       <c r="L27" s="3">
         <v>56</v>
       </c>
-      <c r="M27" s="3">
+      <c r="M27" s="2">
         <v>57</v>
       </c>
-      <c r="N27" s="3">
+      <c r="N27" s="2">
         <v>58</v>
       </c>
-      <c r="O27" s="3">
+      <c r="O27" s="2">
         <v>59</v>
       </c>
-      <c r="P27" s="3">
+      <c r="P27" s="2">
         <v>60</v>
       </c>
-      <c r="Q27" s="3">
+      <c r="Q27" s="2">
         <v>61</v>
       </c>
       <c r="R27" s="3">
@@ -5496,13 +5780,13 @@
       <c r="V27" s="3">
         <v>56</v>
       </c>
-      <c r="W27" s="3">
+      <c r="W27" s="2">
         <v>57</v>
       </c>
       <c r="X27" s="3">
         <v>58</v>
       </c>
-      <c r="Y27" s="2">
+      <c r="Y27" s="3">
         <v>59</v>
       </c>
       <c r="Z27" s="3">
@@ -5517,6 +5801,7 @@
       <c r="AC27" s="3">
         <v>63</v>
       </c>
+      <c r="AD27" s="4"/>
       <c r="AE27" s="3">
         <v>55</v>
       </c>
@@ -5529,13 +5814,13 @@
       <c r="AH27" s="3">
         <v>58</v>
       </c>
-      <c r="AI27" s="2">
+      <c r="AI27" s="3">
         <v>59</v>
       </c>
       <c r="AJ27" s="3">
         <v>60</v>
       </c>
-      <c r="AK27" s="3">
+      <c r="AK27" s="2">
         <v>61</v>
       </c>
       <c r="AL27" s="3">
@@ -5544,8 +5829,9 @@
       <c r="AM27" s="3">
         <v>63</v>
       </c>
-    </row>
-    <row r="28" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN27" s="4"/>
+    </row>
+    <row r="28" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>64</v>
       </c>
@@ -5614,7 +5900,7 @@
       <c r="X28" s="3">
         <v>67</v>
       </c>
-      <c r="Y28" s="2">
+      <c r="Y28" s="3">
         <v>68</v>
       </c>
       <c r="Z28" s="3">
@@ -5629,6 +5915,7 @@
       <c r="AC28" s="3">
         <v>72</v>
       </c>
+      <c r="AD28" s="4"/>
       <c r="AE28" s="3">
         <v>64</v>
       </c>
@@ -5641,7 +5928,7 @@
       <c r="AH28" s="3">
         <v>67</v>
       </c>
-      <c r="AI28" s="2">
+      <c r="AI28" s="3">
         <v>68</v>
       </c>
       <c r="AJ28" s="3">
@@ -5656,8 +5943,9 @@
       <c r="AM28" s="3">
         <v>72</v>
       </c>
-    </row>
-    <row r="29" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN28" s="4"/>
+    </row>
+    <row r="29" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>73</v>
       </c>
@@ -5741,6 +6029,7 @@
       <c r="AC29" s="3">
         <v>81</v>
       </c>
+      <c r="AD29" s="4"/>
       <c r="AE29" s="3">
         <v>73</v>
       </c>
@@ -5768,8 +6057,9 @@
       <c r="AM29" s="3">
         <v>81</v>
       </c>
-    </row>
-    <row r="30" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN29" s="4"/>
+    </row>
+    <row r="30" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -5800,7 +6090,7 @@
       <c r="AB30" s="4"/>
       <c r="AC30" s="4"/>
     </row>
-    <row r="31" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>1</v>
       </c>
@@ -5884,8 +6174,35 @@
       <c r="AC31" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF31" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG31" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH31" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI31" s="3">
+        <v>5</v>
+      </c>
+      <c r="AJ31" s="3">
+        <v>6</v>
+      </c>
+      <c r="AK31" s="3">
+        <v>7</v>
+      </c>
+      <c r="AL31" s="3">
+        <v>8</v>
+      </c>
+      <c r="AM31" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>10</v>
       </c>
@@ -5969,15 +6286,42 @@
       <c r="AC32" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE32" s="3">
+        <v>10</v>
+      </c>
+      <c r="AF32" s="3">
+        <v>11</v>
+      </c>
+      <c r="AG32" s="3">
+        <v>12</v>
+      </c>
+      <c r="AH32" s="3">
+        <v>13</v>
+      </c>
+      <c r="AI32" s="3">
+        <v>14</v>
+      </c>
+      <c r="AJ32" s="3">
+        <v>15</v>
+      </c>
+      <c r="AK32" s="3">
+        <v>16</v>
+      </c>
+      <c r="AL32" s="3">
+        <v>17</v>
+      </c>
+      <c r="AM32" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>19</v>
       </c>
       <c r="B33" s="3">
         <v>20</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>21</v>
       </c>
       <c r="D33" s="3">
@@ -5989,7 +6333,7 @@
       <c r="F33" s="3">
         <v>24</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33" s="2">
         <v>25</v>
       </c>
       <c r="H33" s="3">
@@ -6005,19 +6349,19 @@
       <c r="L33" s="3">
         <v>20</v>
       </c>
-      <c r="M33" s="3">
+      <c r="M33" s="2">
         <v>21</v>
       </c>
-      <c r="N33" s="3">
+      <c r="N33" s="2">
         <v>22</v>
       </c>
-      <c r="O33" s="3">
+      <c r="O33" s="2">
         <v>23</v>
       </c>
-      <c r="P33" s="3">
+      <c r="P33" s="2">
         <v>24</v>
       </c>
-      <c r="Q33" s="3">
+      <c r="Q33" s="2">
         <v>25</v>
       </c>
       <c r="R33" s="3">
@@ -6033,19 +6377,19 @@
       <c r="V33" s="3">
         <v>20</v>
       </c>
-      <c r="W33" s="3">
+      <c r="W33" s="2">
         <v>21</v>
       </c>
-      <c r="X33" s="3">
+      <c r="X33" s="2">
         <v>22</v>
       </c>
-      <c r="Y33" s="3">
+      <c r="Y33" s="2">
         <v>23</v>
       </c>
-      <c r="Z33" s="3">
+      <c r="Z33" s="2">
         <v>24</v>
       </c>
-      <c r="AA33" s="3">
+      <c r="AA33" s="2">
         <v>25</v>
       </c>
       <c r="AB33" s="3">
@@ -6054,15 +6398,42 @@
       <c r="AC33" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE33" s="3">
+        <v>19</v>
+      </c>
+      <c r="AF33" s="3">
+        <v>20</v>
+      </c>
+      <c r="AG33" s="2">
+        <v>21</v>
+      </c>
+      <c r="AH33" s="2">
+        <v>22</v>
+      </c>
+      <c r="AI33" s="2">
+        <v>23</v>
+      </c>
+      <c r="AJ33" s="2">
+        <v>24</v>
+      </c>
+      <c r="AK33" s="2">
+        <v>25</v>
+      </c>
+      <c r="AL33" s="3">
+        <v>26</v>
+      </c>
+      <c r="AM33" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>28</v>
       </c>
       <c r="B34" s="3">
         <v>29</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>30</v>
       </c>
       <c r="D34" s="3">
@@ -6074,7 +6445,7 @@
       <c r="F34" s="3">
         <v>33</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="2">
         <v>34</v>
       </c>
       <c r="H34" s="3">
@@ -6090,7 +6461,7 @@
       <c r="L34" s="3">
         <v>29</v>
       </c>
-      <c r="M34" s="3">
+      <c r="M34" s="2">
         <v>30</v>
       </c>
       <c r="N34" s="3">
@@ -6130,7 +6501,7 @@
       <c r="Z34" s="3">
         <v>33</v>
       </c>
-      <c r="AA34" s="3">
+      <c r="AA34" s="2">
         <v>34</v>
       </c>
       <c r="AB34" s="3">
@@ -6139,15 +6510,42 @@
       <c r="AC34" s="3">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE34" s="3">
+        <v>28</v>
+      </c>
+      <c r="AF34" s="3">
+        <v>29</v>
+      </c>
+      <c r="AG34" s="2">
+        <v>30</v>
+      </c>
+      <c r="AH34" s="3">
+        <v>31</v>
+      </c>
+      <c r="AI34" s="3">
+        <v>32</v>
+      </c>
+      <c r="AJ34" s="3">
+        <v>33</v>
+      </c>
+      <c r="AK34" s="2">
+        <v>34</v>
+      </c>
+      <c r="AL34" s="3">
+        <v>35</v>
+      </c>
+      <c r="AM34" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>37</v>
       </c>
       <c r="B35" s="3">
         <v>38</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>39</v>
       </c>
       <c r="D35" s="3">
@@ -6159,7 +6557,7 @@
       <c r="F35" s="3">
         <v>42</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="2">
         <v>43</v>
       </c>
       <c r="H35" s="3">
@@ -6175,7 +6573,7 @@
       <c r="L35" s="3">
         <v>38</v>
       </c>
-      <c r="M35" s="3">
+      <c r="M35" s="2">
         <v>39</v>
       </c>
       <c r="N35" s="3">
@@ -6215,7 +6613,7 @@
       <c r="Z35" s="3">
         <v>42</v>
       </c>
-      <c r="AA35" s="3">
+      <c r="AA35" s="2">
         <v>43</v>
       </c>
       <c r="AB35" s="3">
@@ -6224,15 +6622,42 @@
       <c r="AC35" s="3">
         <v>45</v>
       </c>
-    </row>
-    <row r="36" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE35" s="3">
+        <v>37</v>
+      </c>
+      <c r="AF35" s="3">
+        <v>38</v>
+      </c>
+      <c r="AG35" s="2">
+        <v>39</v>
+      </c>
+      <c r="AH35" s="3">
+        <v>40</v>
+      </c>
+      <c r="AI35" s="3">
+        <v>41</v>
+      </c>
+      <c r="AJ35" s="3">
+        <v>42</v>
+      </c>
+      <c r="AK35" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL35" s="3">
+        <v>44</v>
+      </c>
+      <c r="AM35" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>46</v>
       </c>
       <c r="B36" s="3">
         <v>47</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>48</v>
       </c>
       <c r="D36" s="3">
@@ -6244,7 +6669,7 @@
       <c r="F36" s="3">
         <v>51</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="2">
         <v>52</v>
       </c>
       <c r="H36" s="3">
@@ -6260,7 +6685,7 @@
       <c r="L36" s="3">
         <v>47</v>
       </c>
-      <c r="M36" s="3">
+      <c r="M36" s="2">
         <v>48</v>
       </c>
       <c r="N36" s="3">
@@ -6300,7 +6725,7 @@
       <c r="Z36" s="3">
         <v>51</v>
       </c>
-      <c r="AA36" s="3">
+      <c r="AA36" s="2">
         <v>52</v>
       </c>
       <c r="AB36" s="3">
@@ -6309,27 +6734,54 @@
       <c r="AC36" s="3">
         <v>54</v>
       </c>
-    </row>
-    <row r="37" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE36" s="3">
+        <v>46</v>
+      </c>
+      <c r="AF36" s="3">
+        <v>47</v>
+      </c>
+      <c r="AG36" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH36" s="3">
+        <v>49</v>
+      </c>
+      <c r="AI36" s="3">
+        <v>50</v>
+      </c>
+      <c r="AJ36" s="3">
+        <v>51</v>
+      </c>
+      <c r="AK36" s="2">
+        <v>52</v>
+      </c>
+      <c r="AL36" s="3">
+        <v>53</v>
+      </c>
+      <c r="AM36" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>55</v>
       </c>
       <c r="B37" s="3">
         <v>56</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>57</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>58</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <v>59</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="2">
         <v>60</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="2">
         <v>61</v>
       </c>
       <c r="H37" s="3">
@@ -6345,19 +6797,19 @@
       <c r="L37" s="3">
         <v>56</v>
       </c>
-      <c r="M37" s="3">
+      <c r="M37" s="2">
         <v>57</v>
       </c>
-      <c r="N37" s="3">
+      <c r="N37" s="2">
         <v>58</v>
       </c>
-      <c r="O37" s="3">
+      <c r="O37" s="2">
         <v>59</v>
       </c>
-      <c r="P37" s="3">
+      <c r="P37" s="2">
         <v>60</v>
       </c>
-      <c r="Q37" s="3">
+      <c r="Q37" s="2">
         <v>61</v>
       </c>
       <c r="R37" s="3">
@@ -6373,19 +6825,19 @@
       <c r="V37" s="3">
         <v>56</v>
       </c>
-      <c r="W37" s="3">
+      <c r="W37" s="2">
         <v>57</v>
       </c>
-      <c r="X37" s="3">
+      <c r="X37" s="2">
         <v>58</v>
       </c>
-      <c r="Y37" s="3">
+      <c r="Y37" s="2">
         <v>59</v>
       </c>
-      <c r="Z37" s="3">
+      <c r="Z37" s="2">
         <v>60</v>
       </c>
-      <c r="AA37" s="3">
+      <c r="AA37" s="2">
         <v>61</v>
       </c>
       <c r="AB37" s="3">
@@ -6394,8 +6846,35 @@
       <c r="AC37" s="3">
         <v>63</v>
       </c>
-    </row>
-    <row r="38" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE37" s="3">
+        <v>55</v>
+      </c>
+      <c r="AF37" s="3">
+        <v>56</v>
+      </c>
+      <c r="AG37" s="2">
+        <v>57</v>
+      </c>
+      <c r="AH37" s="3">
+        <v>58</v>
+      </c>
+      <c r="AI37" s="3">
+        <v>59</v>
+      </c>
+      <c r="AJ37" s="3">
+        <v>60</v>
+      </c>
+      <c r="AK37" s="2">
+        <v>61</v>
+      </c>
+      <c r="AL37" s="3">
+        <v>62</v>
+      </c>
+      <c r="AM37" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>64</v>
       </c>
@@ -6479,8 +6958,35 @@
       <c r="AC38" s="3">
         <v>72</v>
       </c>
-    </row>
-    <row r="39" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE38" s="3">
+        <v>64</v>
+      </c>
+      <c r="AF38" s="3">
+        <v>65</v>
+      </c>
+      <c r="AG38" s="3">
+        <v>66</v>
+      </c>
+      <c r="AH38" s="3">
+        <v>67</v>
+      </c>
+      <c r="AI38" s="3">
+        <v>68</v>
+      </c>
+      <c r="AJ38" s="3">
+        <v>69</v>
+      </c>
+      <c r="AK38" s="3">
+        <v>70</v>
+      </c>
+      <c r="AL38" s="3">
+        <v>71</v>
+      </c>
+      <c r="AM38" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>73</v>
       </c>
@@ -6564,8 +7070,35 @@
       <c r="AC39" s="3">
         <v>81</v>
       </c>
-    </row>
-    <row r="40" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE39" s="3">
+        <v>73</v>
+      </c>
+      <c r="AF39" s="3">
+        <v>74</v>
+      </c>
+      <c r="AG39" s="3">
+        <v>75</v>
+      </c>
+      <c r="AH39" s="3">
+        <v>76</v>
+      </c>
+      <c r="AI39" s="3">
+        <v>77</v>
+      </c>
+      <c r="AJ39" s="3">
+        <v>78</v>
+      </c>
+      <c r="AK39" s="3">
+        <v>79</v>
+      </c>
+      <c r="AL39" s="3">
+        <v>80</v>
+      </c>
+      <c r="AM39" s="3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -6596,9 +7129,1025 @@
       <c r="AB40" s="4"/>
       <c r="AC40" s="4"/>
     </row>
-    <row r="41" spans="1:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>1</v>
+      </c>
+      <c r="B41" s="3">
+        <v>2</v>
+      </c>
+      <c r="C41" s="3">
+        <v>3</v>
+      </c>
+      <c r="D41" s="3">
+        <v>4</v>
+      </c>
+      <c r="E41" s="3">
+        <v>5</v>
+      </c>
+      <c r="F41" s="3">
+        <v>6</v>
+      </c>
+      <c r="G41" s="3">
+        <v>7</v>
+      </c>
+      <c r="H41" s="3">
+        <v>8</v>
+      </c>
+      <c r="I41" s="3">
+        <v>9</v>
+      </c>
+      <c r="J41" s="4"/>
+      <c r="K41" s="3">
+        <v>1</v>
+      </c>
+      <c r="L41" s="3">
+        <v>2</v>
+      </c>
+      <c r="M41" s="3">
+        <v>3</v>
+      </c>
+      <c r="N41" s="3">
+        <v>4</v>
+      </c>
+      <c r="O41" s="3">
+        <v>5</v>
+      </c>
+      <c r="P41" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>7</v>
+      </c>
+      <c r="R41" s="3">
+        <v>8</v>
+      </c>
+      <c r="S41" s="3">
+        <v>9</v>
+      </c>
+      <c r="T41" s="4"/>
+      <c r="U41" s="3">
+        <v>1</v>
+      </c>
+      <c r="V41" s="3">
+        <v>2</v>
+      </c>
+      <c r="W41" s="3">
+        <v>3</v>
+      </c>
+      <c r="X41" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y41" s="3">
+        <v>5</v>
+      </c>
+      <c r="Z41" s="3">
+        <v>6</v>
+      </c>
+      <c r="AA41" s="3">
+        <v>7</v>
+      </c>
+      <c r="AB41" s="3">
+        <v>8</v>
+      </c>
+      <c r="AC41" s="3">
+        <v>9</v>
+      </c>
+      <c r="AE41" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF41" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG41" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH41" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI41" s="3">
+        <v>5</v>
+      </c>
+      <c r="AJ41" s="3">
+        <v>6</v>
+      </c>
+      <c r="AK41" s="3">
+        <v>7</v>
+      </c>
+      <c r="AL41" s="3">
+        <v>8</v>
+      </c>
+      <c r="AM41" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <v>10</v>
+      </c>
+      <c r="B42" s="3">
+        <v>11</v>
+      </c>
+      <c r="C42" s="3">
+        <v>12</v>
+      </c>
+      <c r="D42" s="3">
+        <v>13</v>
+      </c>
+      <c r="E42" s="3">
+        <v>14</v>
+      </c>
+      <c r="F42" s="3">
+        <v>15</v>
+      </c>
+      <c r="G42" s="3">
+        <v>16</v>
+      </c>
+      <c r="H42" s="3">
+        <v>17</v>
+      </c>
+      <c r="I42" s="3">
+        <v>18</v>
+      </c>
+      <c r="J42" s="4"/>
+      <c r="K42" s="3">
+        <v>10</v>
+      </c>
+      <c r="L42" s="3">
+        <v>11</v>
+      </c>
+      <c r="M42" s="3">
+        <v>12</v>
+      </c>
+      <c r="N42" s="3">
+        <v>13</v>
+      </c>
+      <c r="O42" s="3">
+        <v>14</v>
+      </c>
+      <c r="P42" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>16</v>
+      </c>
+      <c r="R42" s="3">
+        <v>17</v>
+      </c>
+      <c r="S42" s="3">
+        <v>18</v>
+      </c>
+      <c r="T42" s="4"/>
+      <c r="U42" s="3">
+        <v>10</v>
+      </c>
+      <c r="V42" s="3">
+        <v>11</v>
+      </c>
+      <c r="W42" s="3">
+        <v>12</v>
+      </c>
+      <c r="X42" s="3">
+        <v>13</v>
+      </c>
+      <c r="Y42" s="3">
+        <v>14</v>
+      </c>
+      <c r="Z42" s="3">
+        <v>15</v>
+      </c>
+      <c r="AA42" s="3">
+        <v>16</v>
+      </c>
+      <c r="AB42" s="3">
+        <v>17</v>
+      </c>
+      <c r="AC42" s="3">
+        <v>18</v>
+      </c>
+      <c r="AE42" s="3">
+        <v>10</v>
+      </c>
+      <c r="AF42" s="3">
+        <v>11</v>
+      </c>
+      <c r="AG42" s="3">
+        <v>12</v>
+      </c>
+      <c r="AH42" s="3">
+        <v>13</v>
+      </c>
+      <c r="AI42" s="3">
+        <v>14</v>
+      </c>
+      <c r="AJ42" s="3">
+        <v>15</v>
+      </c>
+      <c r="AK42" s="3">
+        <v>16</v>
+      </c>
+      <c r="AL42" s="3">
+        <v>17</v>
+      </c>
+      <c r="AM42" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>19</v>
+      </c>
+      <c r="B43" s="3">
+        <v>20</v>
+      </c>
+      <c r="C43" s="2">
+        <v>21</v>
+      </c>
+      <c r="D43" s="3">
+        <v>22</v>
+      </c>
+      <c r="E43" s="2">
+        <v>23</v>
+      </c>
+      <c r="F43" s="3">
+        <v>24</v>
+      </c>
+      <c r="G43" s="2">
+        <v>25</v>
+      </c>
+      <c r="H43" s="3">
+        <v>26</v>
+      </c>
+      <c r="I43" s="3">
+        <v>27</v>
+      </c>
+      <c r="J43" s="4"/>
+      <c r="K43" s="3">
+        <v>19</v>
+      </c>
+      <c r="L43" s="3">
+        <v>20</v>
+      </c>
+      <c r="M43" s="2">
+        <v>21</v>
+      </c>
+      <c r="N43" s="2">
+        <v>22</v>
+      </c>
+      <c r="O43" s="2">
+        <v>23</v>
+      </c>
+      <c r="P43" s="2">
+        <v>24</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>25</v>
+      </c>
+      <c r="R43" s="3">
+        <v>26</v>
+      </c>
+      <c r="S43" s="3">
+        <v>27</v>
+      </c>
+      <c r="T43" s="4"/>
+      <c r="U43" s="3">
+        <v>19</v>
+      </c>
+      <c r="V43" s="3">
+        <v>20</v>
+      </c>
+      <c r="W43" s="2">
+        <v>21</v>
+      </c>
+      <c r="X43" s="2">
+        <v>22</v>
+      </c>
+      <c r="Y43" s="2">
+        <v>23</v>
+      </c>
+      <c r="Z43" s="2">
+        <v>24</v>
+      </c>
+      <c r="AA43" s="2">
+        <v>25</v>
+      </c>
+      <c r="AB43" s="3">
+        <v>26</v>
+      </c>
+      <c r="AC43" s="3">
+        <v>27</v>
+      </c>
+      <c r="AE43" s="3">
+        <v>19</v>
+      </c>
+      <c r="AF43" s="3">
+        <v>20</v>
+      </c>
+      <c r="AG43" s="2">
+        <v>21</v>
+      </c>
+      <c r="AH43" s="2">
+        <v>22</v>
+      </c>
+      <c r="AI43" s="2">
+        <v>23</v>
+      </c>
+      <c r="AJ43" s="2">
+        <v>24</v>
+      </c>
+      <c r="AK43" s="2">
+        <v>25</v>
+      </c>
+      <c r="AL43" s="3">
+        <v>26</v>
+      </c>
+      <c r="AM43" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>28</v>
+      </c>
+      <c r="B44" s="3">
+        <v>29</v>
+      </c>
+      <c r="C44" s="2">
+        <v>30</v>
+      </c>
+      <c r="D44" s="3">
+        <v>31</v>
+      </c>
+      <c r="E44" s="2">
+        <v>32</v>
+      </c>
+      <c r="F44" s="3">
+        <v>33</v>
+      </c>
+      <c r="G44" s="2">
+        <v>34</v>
+      </c>
+      <c r="H44" s="3">
+        <v>35</v>
+      </c>
+      <c r="I44" s="3">
+        <v>36</v>
+      </c>
+      <c r="J44" s="4"/>
+      <c r="K44" s="3">
+        <v>28</v>
+      </c>
+      <c r="L44" s="3">
+        <v>29</v>
+      </c>
+      <c r="M44" s="2">
+        <v>30</v>
+      </c>
+      <c r="N44" s="3">
+        <v>31</v>
+      </c>
+      <c r="O44" s="3">
+        <v>32</v>
+      </c>
+      <c r="P44" s="3">
+        <v>33</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>34</v>
+      </c>
+      <c r="R44" s="3">
+        <v>35</v>
+      </c>
+      <c r="S44" s="3">
+        <v>36</v>
+      </c>
+      <c r="T44" s="4"/>
+      <c r="U44" s="3">
+        <v>28</v>
+      </c>
+      <c r="V44" s="3">
+        <v>29</v>
+      </c>
+      <c r="W44" s="3">
+        <v>30</v>
+      </c>
+      <c r="X44" s="3">
+        <v>31</v>
+      </c>
+      <c r="Y44" s="3">
+        <v>32</v>
+      </c>
+      <c r="Z44" s="3">
+        <v>33</v>
+      </c>
+      <c r="AA44" s="2">
+        <v>34</v>
+      </c>
+      <c r="AB44" s="3">
+        <v>35</v>
+      </c>
+      <c r="AC44" s="3">
+        <v>36</v>
+      </c>
+      <c r="AE44" s="3">
+        <v>28</v>
+      </c>
+      <c r="AF44" s="3">
+        <v>29</v>
+      </c>
+      <c r="AG44" s="2">
+        <v>30</v>
+      </c>
+      <c r="AH44" s="3">
+        <v>31</v>
+      </c>
+      <c r="AI44" s="2">
+        <v>32</v>
+      </c>
+      <c r="AJ44" s="3">
+        <v>33</v>
+      </c>
+      <c r="AK44" s="2">
+        <v>34</v>
+      </c>
+      <c r="AL44" s="3">
+        <v>35</v>
+      </c>
+      <c r="AM44" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>37</v>
+      </c>
+      <c r="B45" s="3">
+        <v>38</v>
+      </c>
+      <c r="C45" s="2">
+        <v>39</v>
+      </c>
+      <c r="D45" s="3">
+        <v>40</v>
+      </c>
+      <c r="E45" s="2">
+        <v>41</v>
+      </c>
+      <c r="F45" s="3">
+        <v>42</v>
+      </c>
+      <c r="G45" s="2">
+        <v>43</v>
+      </c>
+      <c r="H45" s="3">
+        <v>44</v>
+      </c>
+      <c r="I45" s="3">
+        <v>45</v>
+      </c>
+      <c r="J45" s="4"/>
+      <c r="K45" s="3">
+        <v>37</v>
+      </c>
+      <c r="L45" s="3">
+        <v>38</v>
+      </c>
+      <c r="M45" s="2">
+        <v>39</v>
+      </c>
+      <c r="N45" s="2">
+        <v>40</v>
+      </c>
+      <c r="O45" s="2">
+        <v>41</v>
+      </c>
+      <c r="P45" s="2">
+        <v>42</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>43</v>
+      </c>
+      <c r="R45" s="3">
+        <v>44</v>
+      </c>
+      <c r="S45" s="3">
+        <v>45</v>
+      </c>
+      <c r="T45" s="4"/>
+      <c r="U45" s="3">
+        <v>37</v>
+      </c>
+      <c r="V45" s="3">
+        <v>38</v>
+      </c>
+      <c r="W45" s="2">
+        <v>39</v>
+      </c>
+      <c r="X45" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y45" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z45" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA45" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB45" s="3">
+        <v>44</v>
+      </c>
+      <c r="AC45" s="3">
+        <v>45</v>
+      </c>
+      <c r="AE45" s="3">
+        <v>37</v>
+      </c>
+      <c r="AF45" s="3">
+        <v>38</v>
+      </c>
+      <c r="AG45" s="2">
+        <v>39</v>
+      </c>
+      <c r="AH45" s="3">
+        <v>40</v>
+      </c>
+      <c r="AI45" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ45" s="3">
+        <v>42</v>
+      </c>
+      <c r="AK45" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL45" s="3">
+        <v>44</v>
+      </c>
+      <c r="AM45" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>46</v>
+      </c>
+      <c r="B46" s="3">
+        <v>47</v>
+      </c>
+      <c r="C46" s="2">
+        <v>48</v>
+      </c>
+      <c r="D46" s="3">
+        <v>49</v>
+      </c>
+      <c r="E46" s="2">
+        <v>50</v>
+      </c>
+      <c r="F46" s="3">
+        <v>51</v>
+      </c>
+      <c r="G46" s="2">
+        <v>52</v>
+      </c>
+      <c r="H46" s="3">
+        <v>53</v>
+      </c>
+      <c r="I46" s="3">
+        <v>54</v>
+      </c>
+      <c r="J46" s="4"/>
+      <c r="K46" s="3">
+        <v>46</v>
+      </c>
+      <c r="L46" s="3">
+        <v>47</v>
+      </c>
+      <c r="M46" s="2">
+        <v>48</v>
+      </c>
+      <c r="N46" s="3">
+        <v>49</v>
+      </c>
+      <c r="O46" s="3">
+        <v>50</v>
+      </c>
+      <c r="P46" s="3">
+        <v>51</v>
+      </c>
+      <c r="Q46" s="3">
+        <v>52</v>
+      </c>
+      <c r="R46" s="3">
+        <v>53</v>
+      </c>
+      <c r="S46" s="3">
+        <v>54</v>
+      </c>
+      <c r="T46" s="4"/>
+      <c r="U46" s="3">
+        <v>46</v>
+      </c>
+      <c r="V46" s="3">
+        <v>47</v>
+      </c>
+      <c r="W46" s="3">
+        <v>48</v>
+      </c>
+      <c r="X46" s="3">
+        <v>49</v>
+      </c>
+      <c r="Y46" s="3">
+        <v>50</v>
+      </c>
+      <c r="Z46" s="3">
+        <v>51</v>
+      </c>
+      <c r="AA46" s="2">
+        <v>52</v>
+      </c>
+      <c r="AB46" s="3">
+        <v>53</v>
+      </c>
+      <c r="AC46" s="3">
+        <v>54</v>
+      </c>
+      <c r="AE46" s="3">
+        <v>46</v>
+      </c>
+      <c r="AF46" s="3">
+        <v>47</v>
+      </c>
+      <c r="AG46" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH46" s="3">
+        <v>49</v>
+      </c>
+      <c r="AI46" s="2">
+        <v>50</v>
+      </c>
+      <c r="AJ46" s="3">
+        <v>51</v>
+      </c>
+      <c r="AK46" s="2">
+        <v>52</v>
+      </c>
+      <c r="AL46" s="3">
+        <v>53</v>
+      </c>
+      <c r="AM46" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>55</v>
+      </c>
+      <c r="B47" s="3">
+        <v>56</v>
+      </c>
+      <c r="C47" s="2">
+        <v>57</v>
+      </c>
+      <c r="D47" s="2">
+        <v>58</v>
+      </c>
+      <c r="E47" s="2">
+        <v>59</v>
+      </c>
+      <c r="F47" s="2">
+        <v>60</v>
+      </c>
+      <c r="G47" s="2">
+        <v>61</v>
+      </c>
+      <c r="H47" s="3">
+        <v>62</v>
+      </c>
+      <c r="I47" s="3">
+        <v>63</v>
+      </c>
+      <c r="J47" s="4"/>
+      <c r="K47" s="3">
+        <v>55</v>
+      </c>
+      <c r="L47" s="3">
+        <v>56</v>
+      </c>
+      <c r="M47" s="2">
+        <v>57</v>
+      </c>
+      <c r="N47" s="2">
+        <v>58</v>
+      </c>
+      <c r="O47" s="2">
+        <v>59</v>
+      </c>
+      <c r="P47" s="2">
+        <v>60</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>61</v>
+      </c>
+      <c r="R47" s="3">
+        <v>62</v>
+      </c>
+      <c r="S47" s="3">
+        <v>63</v>
+      </c>
+      <c r="T47" s="4"/>
+      <c r="U47" s="3">
+        <v>55</v>
+      </c>
+      <c r="V47" s="3">
+        <v>56</v>
+      </c>
+      <c r="W47" s="2">
+        <v>57</v>
+      </c>
+      <c r="X47" s="2">
+        <v>58</v>
+      </c>
+      <c r="Y47" s="2">
+        <v>59</v>
+      </c>
+      <c r="Z47" s="2">
+        <v>60</v>
+      </c>
+      <c r="AA47" s="2">
+        <v>61</v>
+      </c>
+      <c r="AB47" s="3">
+        <v>62</v>
+      </c>
+      <c r="AC47" s="3">
+        <v>63</v>
+      </c>
+      <c r="AE47" s="3">
+        <v>55</v>
+      </c>
+      <c r="AF47" s="3">
+        <v>56</v>
+      </c>
+      <c r="AG47" s="2">
+        <v>57</v>
+      </c>
+      <c r="AH47" s="3">
+        <v>58</v>
+      </c>
+      <c r="AI47" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ47" s="3">
+        <v>60</v>
+      </c>
+      <c r="AK47" s="2">
+        <v>61</v>
+      </c>
+      <c r="AL47" s="3">
+        <v>62</v>
+      </c>
+      <c r="AM47" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>64</v>
+      </c>
+      <c r="B48" s="3">
+        <v>65</v>
+      </c>
+      <c r="C48" s="3">
+        <v>66</v>
+      </c>
+      <c r="D48" s="3">
+        <v>67</v>
+      </c>
+      <c r="E48" s="3">
+        <v>68</v>
+      </c>
+      <c r="F48" s="3">
+        <v>69</v>
+      </c>
+      <c r="G48" s="3">
+        <v>70</v>
+      </c>
+      <c r="H48" s="3">
+        <v>71</v>
+      </c>
+      <c r="I48" s="3">
+        <v>72</v>
+      </c>
+      <c r="J48" s="4"/>
+      <c r="K48" s="3">
+        <v>64</v>
+      </c>
+      <c r="L48" s="3">
+        <v>65</v>
+      </c>
+      <c r="M48" s="3">
+        <v>66</v>
+      </c>
+      <c r="N48" s="3">
+        <v>67</v>
+      </c>
+      <c r="O48" s="3">
+        <v>68</v>
+      </c>
+      <c r="P48" s="3">
+        <v>69</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>70</v>
+      </c>
+      <c r="R48" s="3">
+        <v>71</v>
+      </c>
+      <c r="S48" s="3">
+        <v>72</v>
+      </c>
+      <c r="T48" s="4"/>
+      <c r="U48" s="3">
+        <v>64</v>
+      </c>
+      <c r="V48" s="3">
+        <v>65</v>
+      </c>
+      <c r="W48" s="3">
+        <v>66</v>
+      </c>
+      <c r="X48" s="3">
+        <v>67</v>
+      </c>
+      <c r="Y48" s="3">
+        <v>68</v>
+      </c>
+      <c r="Z48" s="3">
+        <v>69</v>
+      </c>
+      <c r="AA48" s="3">
+        <v>70</v>
+      </c>
+      <c r="AB48" s="3">
+        <v>71</v>
+      </c>
+      <c r="AC48" s="3">
+        <v>72</v>
+      </c>
+      <c r="AE48" s="3">
+        <v>64</v>
+      </c>
+      <c r="AF48" s="3">
+        <v>65</v>
+      </c>
+      <c r="AG48" s="3">
+        <v>66</v>
+      </c>
+      <c r="AH48" s="3">
+        <v>67</v>
+      </c>
+      <c r="AI48" s="3">
+        <v>68</v>
+      </c>
+      <c r="AJ48" s="3">
+        <v>69</v>
+      </c>
+      <c r="AK48" s="3">
+        <v>70</v>
+      </c>
+      <c r="AL48" s="3">
+        <v>71</v>
+      </c>
+      <c r="AM48" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>73</v>
+      </c>
+      <c r="B49" s="3">
+        <v>74</v>
+      </c>
+      <c r="C49" s="3">
+        <v>75</v>
+      </c>
+      <c r="D49" s="3">
+        <v>76</v>
+      </c>
+      <c r="E49" s="3">
+        <v>77</v>
+      </c>
+      <c r="F49" s="3">
+        <v>78</v>
+      </c>
+      <c r="G49" s="3">
+        <v>79</v>
+      </c>
+      <c r="H49" s="3">
+        <v>80</v>
+      </c>
+      <c r="I49" s="3">
+        <v>81</v>
+      </c>
+      <c r="J49" s="4"/>
+      <c r="K49" s="3">
+        <v>73</v>
+      </c>
+      <c r="L49" s="3">
+        <v>74</v>
+      </c>
+      <c r="M49" s="3">
+        <v>75</v>
+      </c>
+      <c r="N49" s="3">
+        <v>76</v>
+      </c>
+      <c r="O49" s="3">
+        <v>77</v>
+      </c>
+      <c r="P49" s="3">
+        <v>78</v>
+      </c>
+      <c r="Q49" s="3">
+        <v>79</v>
+      </c>
+      <c r="R49" s="3">
+        <v>80</v>
+      </c>
+      <c r="S49" s="3">
+        <v>81</v>
+      </c>
+      <c r="T49" s="4"/>
+      <c r="U49" s="3">
+        <v>73</v>
+      </c>
+      <c r="V49" s="3">
+        <v>74</v>
+      </c>
+      <c r="W49" s="3">
+        <v>75</v>
+      </c>
+      <c r="X49" s="3">
+        <v>76</v>
+      </c>
+      <c r="Y49" s="3">
+        <v>77</v>
+      </c>
+      <c r="Z49" s="3">
+        <v>78</v>
+      </c>
+      <c r="AA49" s="3">
+        <v>79</v>
+      </c>
+      <c r="AB49" s="3">
+        <v>80</v>
+      </c>
+      <c r="AC49" s="3">
+        <v>81</v>
+      </c>
+      <c r="AE49" s="3">
+        <v>73</v>
+      </c>
+      <c r="AF49" s="3">
+        <v>74</v>
+      </c>
+      <c r="AG49" s="3">
+        <v>75</v>
+      </c>
+      <c r="AH49" s="3">
+        <v>76</v>
+      </c>
+      <c r="AI49" s="3">
+        <v>77</v>
+      </c>
+      <c r="AJ49" s="3">
+        <v>78</v>
+      </c>
+      <c r="AK49" s="3">
+        <v>79</v>
+      </c>
+      <c r="AL49" s="3">
+        <v>80</v>
+      </c>
+      <c r="AM49" s="3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>